<commit_message>
Update header config to match new sheet
</commit_message>
<xml_diff>
--- a/spec/fixtures/Find_Row_Sheet.xlsx
+++ b/spec/fixtures/Find_Row_Sheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>a</t>
   </si>
@@ -33,128 +33,107 @@
     <t>abab</t>
   </si>
   <si>
-    <t>image title</t>
-  </si>
-  <si>
-    <t>url to catalog</t>
-  </si>
-  <si>
-    <t>image type</t>
-  </si>
-  <si>
-    <t>copy:call number</t>
-  </si>
-  <si>
-    <t>copy:volume number</t>
-  </si>
-  <si>
-    <t>copy:current repository</t>
-  </si>
-  <si>
-    <t>copy:current collection</t>
-  </si>
-  <si>
-    <t>copy:author</t>
-  </si>
-  <si>
-    <t>copy:title</t>
-  </si>
-  <si>
-    <t>copy:place of publication</t>
-  </si>
-  <si>
-    <t>copy:date of publication</t>
-  </si>
-  <si>
-    <t>copy:printer/publisher</t>
-  </si>
-  <si>
-    <t>evidence:location in book</t>
-  </si>
-  <si>
-    <t>evidence:format</t>
-  </si>
-  <si>
-    <t>evidence:type</t>
-  </si>
-  <si>
-    <t>evidence:transcription</t>
-  </si>
-  <si>
-    <t>evidence:individual associated name</t>
-  </si>
-  <si>
-    <t>evidence:organization associated name</t>
-  </si>
-  <si>
-    <t>evidence:family associated name</t>
-  </si>
-  <si>
-    <t>evidence:description</t>
-  </si>
-  <si>
-    <t>evidence:status</t>
-  </si>
-  <si>
-    <t>id:date</t>
-  </si>
-  <si>
-    <t>id:place</t>
-  </si>
-  <si>
-    <t>id:individual:owner</t>
-  </si>
-  <si>
-    <t>id:organization:owner</t>
-  </si>
-  <si>
-    <t>id:individual:donor</t>
-  </si>
-  <si>
-    <t>id:organization:donor</t>
-  </si>
-  <si>
-    <t>id:individual:recipient</t>
-  </si>
-  <si>
-    <t>id:organization:recipient</t>
-  </si>
-  <si>
-    <t>id:individual:seller</t>
-  </si>
-  <si>
-    <t>id:organization:seller</t>
-  </si>
-  <si>
-    <t>id:individual:selling agent</t>
-  </si>
-  <si>
-    <t>id:organization:selling agent</t>
-  </si>
-  <si>
-    <t>id:individual:buyer</t>
-  </si>
-  <si>
-    <t>id:organization:buyer</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>evidence:associated date</t>
-  </si>
-  <si>
-    <t>evidence:associated place</t>
-  </si>
-  <si>
-    <t>evidence:creator</t>
+    <t>image file name</t>
+  </si>
+  <si>
+    <t>URL to catalog</t>
+  </si>
+  <si>
+    <t>copy: current repository</t>
+  </si>
+  <si>
+    <t>copy: call number/shelf mark</t>
+  </si>
+  <si>
+    <t>copy: volume number</t>
+  </si>
+  <si>
+    <t>evidence: location in book</t>
+  </si>
+  <si>
+    <t>evidence: image category</t>
+  </si>
+  <si>
+    <t>evidence: format</t>
+  </si>
+  <si>
+    <t>evidence: content type</t>
+  </si>
+  <si>
+    <t>copy: current collection</t>
+  </si>
+  <si>
+    <t>copy: author</t>
+  </si>
+  <si>
+    <t>copy: title</t>
+  </si>
+  <si>
+    <t>copy: place of publication</t>
+  </si>
+  <si>
+    <t>copy: date of publication</t>
+  </si>
+  <si>
+    <t>copy: printer/publisher</t>
+  </si>
+  <si>
+    <t>evidence: transcription</t>
+  </si>
+  <si>
+    <t>evidence: associated name</t>
+  </si>
+  <si>
+    <t>evidence: associated date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evidence: associated place </t>
+  </si>
+  <si>
+    <t>evidence: description</t>
+  </si>
+  <si>
+    <t>evidence: reference citation</t>
+  </si>
+  <si>
+    <t>evidence: comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id: date </t>
+  </si>
+  <si>
+    <t>id: place</t>
+  </si>
+  <si>
+    <t>id: owner</t>
+  </si>
+  <si>
+    <t>id: donor</t>
+  </si>
+  <si>
+    <t>id: recipient</t>
+  </si>
+  <si>
+    <t>id: seller</t>
+  </si>
+  <si>
+    <t>id: selling agent</t>
+  </si>
+  <si>
+    <t>id: buyer</t>
+  </si>
+  <si>
+    <t>id: binder</t>
+  </si>
+  <si>
+    <t>id: viaf authority link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -162,13 +141,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,8 +209,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,147 +549,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM5"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AF1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:39">
-      <c r="A1" t="s">
+    <row r="1" spans="1:32">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T1" t="s">
-        <v>40</v>
-      </c>
-      <c r="U1" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="T1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="U1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="V1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="W1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="X1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="Y1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="Z1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AA1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AB1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AC1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AD1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:32">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
         <v>3</v>
       </c>

</xml_diff>